<commit_message>
logic in search and create new migration with new seed data
</commit_message>
<xml_diff>
--- a/HR_Sys/wwwroot/files/C3B82020.xlsx
+++ b/HR_Sys/wwwroot/files/C3B82020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hady Salah\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9314B967-D83B-40C2-A928-597B33070A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2D6207-8FDF-4931-A92D-79DFA43519DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{174A33C0-DDA3-48E5-961B-7DCCE8371C30}"/>
   </bookViews>
@@ -34,13 +34,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>attendance time</t>
+  </si>
+  <si>
+    <t>departure time</t>
+  </si>
+  <si>
+    <t>attendance Date</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -68,9 +89,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -385,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F838758-876F-4352-ADA2-F9CDA793C387}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -398,17 +422,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
-        <v>44542.333333333336</v>
-      </c>
-      <c r="C1" s="1">
-        <v>44542.625</v>
-      </c>
-      <c r="D1" s="1">
-        <v>44519</v>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -422,48 +446,126 @@
         <v>44542.625</v>
       </c>
       <c r="D2" s="1">
-        <v>44520</v>
+        <v>44502</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C3" s="1">
+        <v>44542.708333333336</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>44542.333333333336</v>
+      </c>
+      <c r="C4" s="1">
+        <v>44542.666666666664</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>44542.416666666664</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44542.708333333336</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1">
+        <v>44542.416666666664</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>44542.416666666664</v>
+      </c>
+      <c r="C7" s="1">
+        <v>44542.666666666664</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>44542.375</v>
+      </c>
+      <c r="C8" s="1">
+        <v>44542.666666666664</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44502</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1">
+        <v>44542.375</v>
+      </c>
+      <c r="C9" s="1">
+        <v>44542.708333333336</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1">
+        <v>44542.375</v>
+      </c>
+      <c r="C10" s="1">
+        <v>44542.625</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44502</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>